<commit_message>
Implement programming questions functionality
</commit_message>
<xml_diff>
--- a/android/assets/Resources/MCQ/ProgrammingQ/ProgrammingQ-Database.xlsx
+++ b/android/assets/Resources/MCQ/ProgrammingQ/ProgrammingQ-Database.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmate\OneDrive\Documents\School\2nd Year\2nd Sem\CMSC 123 (DSA 2)\HackerGame\android\assets\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmate\OneDrive\Documents\School\2nd Year\Midyear\CMSC 13 (PROGRAMMING PARADIGMS)\TheProgrammer'sAtlas\android\assets\Resources\MCQ\ProgrammingQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1185ADE0-8229-4ACF-8140-CEAA8921FAEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCE771A-17C4-4E64-A659-F927BBC57C92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22170" yWindow="720" windowWidth="6630" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
   <si>
     <t>Question Number</t>
   </si>
@@ -38,18 +38,6 @@
     <t>Question</t>
   </si>
   <si>
-    <t>Choice One</t>
-  </si>
-  <si>
-    <t>Choice Two</t>
-  </si>
-  <si>
-    <t>Choice Three</t>
-  </si>
-  <si>
-    <t>Choice Four</t>
-  </si>
-  <si>
     <t>Correct Choice</t>
   </si>
   <si>
@@ -59,24 +47,9 @@
     <t>Difficulty</t>
   </si>
   <si>
-    <t>Graph Theory: A Review</t>
-  </si>
-  <si>
     <t>Consider a small country with five cities: A, B, C, D, E. There are six flights: A-B, A-C, A-E, B-D, C-D, C-E. Can one get from A to D with only one step?</t>
   </si>
   <si>
-    <t>Yes, there is a direct flight from A to D.</t>
-  </si>
-  <si>
-    <t>No, there is no direct flight from A to D.</t>
-  </si>
-  <si>
-    <t>Maybe, there may be a direct flight from A to D.</t>
-  </si>
-  <si>
-    <t>Yes, there is a direct flight from A to C.</t>
-  </si>
-  <si>
     <t>Yes, one can fly through B or C.</t>
   </si>
   <si>
@@ -194,66 +167,9 @@
     <t>connected</t>
   </si>
   <si>
-    <t>A ______ in a graph is a sequence of edges, such that each edge (except for the first one) starts with a vertex where the previous edge ended.</t>
-  </si>
-  <si>
-    <t>walk</t>
-  </si>
-  <si>
-    <t>A ______ is a walk where all edges are distinct.</t>
-  </si>
-  <si>
-    <t>directed walk</t>
-  </si>
-  <si>
-    <t>connected walk</t>
-  </si>
-  <si>
-    <t>A ______ is a walk where all vertices are distinct.</t>
-  </si>
-  <si>
-    <t>simple path</t>
-  </si>
-  <si>
-    <t>simple walk</t>
-  </si>
-  <si>
-    <t>simple cycle</t>
-  </si>
-  <si>
-    <t>complicated walk</t>
-  </si>
-  <si>
-    <t>A ______ in a graph is a path whose vertex is the same as the last one.</t>
-  </si>
-  <si>
-    <t>component</t>
-  </si>
-  <si>
-    <t>A ______ is a cycle where all vertices except for the first one are distinct.</t>
-  </si>
-  <si>
-    <t>distinct cycle</t>
-  </si>
-  <si>
-    <t>complex cycle</t>
-  </si>
-  <si>
-    <t>complicated cycle</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>A</t>
   </si>
   <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>C</t>
-  </si>
-  <si>
     <t>EASY</t>
   </si>
   <si>
@@ -273,6 +189,45 @@
   </si>
   <si>
     <t>GT9.png</t>
+  </si>
+  <si>
+    <t>C++</t>
+  </si>
+  <si>
+    <t>PYTHON</t>
+  </si>
+  <si>
+    <t>VERY EASY</t>
+  </si>
+  <si>
+    <t>VERY HARD</t>
+  </si>
+  <si>
+    <t>ve_c++_question.png</t>
+  </si>
+  <si>
+    <t>Choice A</t>
+  </si>
+  <si>
+    <t>Choice B</t>
+  </si>
+  <si>
+    <t>Choice C</t>
+  </si>
+  <si>
+    <t>Choice D</t>
+  </si>
+  <si>
+    <t>ve_c++_choiceA.png</t>
+  </si>
+  <si>
+    <t>ve_c++_choiceB.png</t>
+  </si>
+  <si>
+    <t>ve_c++_choiceC.png</t>
+  </si>
+  <si>
+    <t>ve_c++_choiceD.png</t>
   </si>
 </sst>
 </file>
@@ -624,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J16"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -643,25 +598,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -669,28 +624,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>12</v>
+        <v>63</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="J2" t="s">
-        <v>75</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -698,28 +653,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" t="s">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="J3" t="s">
-        <v>75</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -727,28 +682,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
       <c r="G4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="J4" t="s">
-        <v>75</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -756,31 +711,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="G5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>78</v>
+        <v>50</v>
       </c>
       <c r="J5" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -788,31 +743,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="G6" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H6" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
       <c r="J6" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -820,31 +775,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="D7" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="E7" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="G7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="H7" t="s">
-        <v>73</v>
+        <v>46</v>
       </c>
       <c r="I7" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="J7" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -852,28 +807,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D8" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="H8" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -881,28 +836,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C9" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E9" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" t="s">
+        <v>39</v>
+      </c>
+      <c r="H9" t="s">
         <v>46</v>
       </c>
-      <c r="F9" t="s">
-        <v>47</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>48</v>
-      </c>
-      <c r="H9" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -910,10 +865,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -928,13 +883,13 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="I10" t="s">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="J10" t="s">
-        <v>76</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -942,173 +897,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>55</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="D11" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="F11" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="G11" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="H11" t="s">
-        <v>74</v>
+        <v>46</v>
       </c>
       <c r="J11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
-      </c>
-      <c r="E12" t="s">
-        <v>56</v>
-      </c>
-      <c r="F12" t="s">
-        <v>42</v>
-      </c>
-      <c r="G12" t="s">
-        <v>43</v>
-      </c>
-      <c r="H12" t="s">
-        <v>71</v>
-      </c>
-      <c r="J12" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
         <v>57</v>
-      </c>
-      <c r="D13" t="s">
-        <v>41</v>
-      </c>
-      <c r="E13" t="s">
-        <v>40</v>
-      </c>
-      <c r="F13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" t="s">
-        <v>59</v>
-      </c>
-      <c r="H13" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" t="s">
-        <v>60</v>
-      </c>
-      <c r="D14" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="F14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-      <c r="H14" t="s">
-        <v>72</v>
-      </c>
-      <c r="J14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>10</v>
-      </c>
-      <c r="C15" t="s">
-        <v>65</v>
-      </c>
-      <c r="D15" t="s">
-        <v>41</v>
-      </c>
-      <c r="E15" t="s">
-        <v>66</v>
-      </c>
-      <c r="F15" t="s">
-        <v>56</v>
-      </c>
-      <c r="G15" t="s">
-        <v>43</v>
-      </c>
-      <c r="H15" t="s">
-        <v>72</v>
-      </c>
-      <c r="J15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" t="s">
-        <v>67</v>
-      </c>
-      <c r="D16" t="s">
-        <v>68</v>
-      </c>
-      <c r="E16" t="s">
-        <v>63</v>
-      </c>
-      <c r="F16" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" t="s">
-        <v>70</v>
-      </c>
-      <c r="H16" t="s">
-        <v>71</v>
-      </c>
-      <c r="J16" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add easy, medium, and hard images
</commit_message>
<xml_diff>
--- a/android/assets/Resources/MCQ/ProgrammingQ/ProgrammingQ-Database.xlsx
+++ b/android/assets/Resources/MCQ/ProgrammingQ/ProgrammingQ-Database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cmate\OneDrive\Documents\School\2nd Year\Midyear\CMSC 13 (PROGRAMMING PARADIGMS)\TheProgrammer'sAtlas\android\assets\Resources\MCQ\ProgrammingQ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDCE771A-17C4-4E64-A659-F927BBC57C92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{578E07EB-A2DE-498F-87A4-6E5025C31C7C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22170" yWindow="720" windowWidth="6630" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14235" yWindow="1065" windowWidth="14925" windowHeight="12690" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="68">
   <si>
     <t>Question Number</t>
   </si>
@@ -47,33 +47,6 @@
     <t>Difficulty</t>
   </si>
   <si>
-    <t>Consider a small country with five cities: A, B, C, D, E. There are six flights: A-B, A-C, A-E, B-D, C-D, C-E. Can one get from A to D with only one step?</t>
-  </si>
-  <si>
-    <t>Yes, one can fly through B or C.</t>
-  </si>
-  <si>
-    <t>No, all the paths from A to D have exactly two steps.</t>
-  </si>
-  <si>
-    <t>Yes, one can fly through E.</t>
-  </si>
-  <si>
-    <t>No, all the paths from A to D have exactly three steps.</t>
-  </si>
-  <si>
-    <t>Consider a small country with five cities: A, B, C, D, E. There are six flights: A-B, A-C, A-E, B-D, C-D, C-E. Can one get from A to D with exactly two steps?</t>
-  </si>
-  <si>
-    <t>Yes, one can stop at B and C.</t>
-  </si>
-  <si>
-    <t>Yes, one can stop at B and E.</t>
-  </si>
-  <si>
-    <t>Yes, one can stop at E and C.</t>
-  </si>
-  <si>
     <t>A Graph G = (V, E). V is a set of Vertices/Nodes and E is the set of Edges. How many vertices does the graph shown below have?</t>
   </si>
   <si>
@@ -228,6 +201,36 @@
   </si>
   <si>
     <t>ve_c++_choiceD.png</t>
+  </si>
+  <si>
+    <t>e_c++_question.png</t>
+  </si>
+  <si>
+    <t>e_c++_choiceA.png</t>
+  </si>
+  <si>
+    <t>e_c++_choiceB.png</t>
+  </si>
+  <si>
+    <t>e_c++_choiceC.png</t>
+  </si>
+  <si>
+    <t>e_c++_choiceD.png</t>
+  </si>
+  <si>
+    <t>m_c++_question.png</t>
+  </si>
+  <si>
+    <t>m_c++_choiceA.png</t>
+  </si>
+  <si>
+    <t>m_c++_choiceB.png</t>
+  </si>
+  <si>
+    <t>m_c++_choiceC.png</t>
+  </si>
+  <si>
+    <t>m_c++_choiceD.png</t>
   </si>
 </sst>
 </file>
@@ -582,7 +585,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,16 +601,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="E1" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -624,28 +627,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
         <v>54</v>
       </c>
-      <c r="C2" t="s">
-        <v>58</v>
-      </c>
-      <c r="D2" t="s">
-        <v>63</v>
-      </c>
       <c r="E2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="G2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="H2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J2" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -653,28 +656,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>59</v>
       </c>
       <c r="E3" t="s">
-        <v>8</v>
+        <v>60</v>
       </c>
       <c r="F3" t="s">
-        <v>9</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J3" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -682,28 +685,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>65</v>
       </c>
       <c r="F4" t="s">
-        <v>10</v>
+        <v>66</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>67</v>
       </c>
       <c r="H4" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -711,31 +714,31 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E5" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="F5" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="H5" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="J5" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -743,31 +746,31 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="C6" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="D6" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="E6" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F6" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="G6" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="J6" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -775,31 +778,31 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="E7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="G7" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="J7" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -807,28 +810,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D8" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="H8" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -836,28 +839,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="E9" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" t="s">
         <v>37</v>
       </c>
-      <c r="F9" t="s">
-        <v>38</v>
-      </c>
-      <c r="G9" t="s">
+      <c r="J9" t="s">
         <v>39</v>
-      </c>
-      <c r="H9" t="s">
-        <v>46</v>
-      </c>
-      <c r="J9" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -865,10 +868,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C10" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D10">
         <v>5</v>
@@ -883,13 +886,13 @@
         <v>4</v>
       </c>
       <c r="H10" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="I10" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="J10" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -897,28 +900,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="C11" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="D11" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="E11" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="F11" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="G11" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="J11" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>